<commit_message>
Automation test suit for language and skill feature of Mars
</commit_message>
<xml_diff>
--- a/Test cases for Mars Application.xlsx
+++ b/Test cases for Mars Application.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MVP studio\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MVP studio\MarsPortal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{673F9763-7AF2-4725-A9EB-D85FFE29605F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4074CCE-AF1A-435E-BA31-58D645D92F32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{48190CAB-6ADD-4050-A54D-47863BE9F7EB}"/>
   </bookViews>
@@ -17,7 +17,6 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -894,9 +893,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -906,10 +902,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
@@ -1239,8 +1238,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7028D3FA-8733-4A07-B51B-54A3265D66B8}">
   <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1387,7 +1386,7 @@
       </c>
     </row>
     <row r="5" spans="1:10" ht="105" x14ac:dyDescent="0.25">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="15" t="s">
         <v>14</v>
       </c>
       <c r="B5" s="13" t="s">
@@ -1419,8 +1418,8 @@
       </c>
     </row>
     <row r="6" spans="1:10" ht="180" x14ac:dyDescent="0.25">
-      <c r="A6" s="17"/>
-      <c r="B6" s="14"/>
+      <c r="A6" s="16"/>
+      <c r="B6" s="18"/>
       <c r="C6" s="3" t="s">
         <v>26</v>
       </c>
@@ -1447,8 +1446,8 @@
       </c>
     </row>
     <row r="7" spans="1:10" ht="90" x14ac:dyDescent="0.25">
-      <c r="A7" s="18"/>
-      <c r="B7" s="15"/>
+      <c r="A7" s="19"/>
+      <c r="B7" s="14"/>
       <c r="C7" s="3" t="s">
         <v>31</v>
       </c>
@@ -1473,7 +1472,7 @@
       </c>
     </row>
     <row r="8" spans="1:10" ht="105" x14ac:dyDescent="0.25">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="15" t="s">
         <v>92</v>
       </c>
       <c r="B8" s="13" t="s">
@@ -1505,8 +1504,8 @@
       </c>
     </row>
     <row r="9" spans="1:10" ht="90" x14ac:dyDescent="0.25">
-      <c r="A9" s="17"/>
-      <c r="B9" s="14"/>
+      <c r="A9" s="16"/>
+      <c r="B9" s="18"/>
       <c r="C9" s="3" t="s">
         <v>38</v>
       </c>
@@ -1531,8 +1530,8 @@
       </c>
     </row>
     <row r="10" spans="1:10" ht="90" x14ac:dyDescent="0.25">
-      <c r="A10" s="18"/>
-      <c r="B10" s="15"/>
+      <c r="A10" s="19"/>
+      <c r="B10" s="14"/>
       <c r="C10" s="3" t="s">
         <v>42</v>
       </c>
@@ -1557,7 +1556,7 @@
       </c>
     </row>
     <row r="11" spans="1:10" ht="105" x14ac:dyDescent="0.25">
-      <c r="A11" s="16" t="s">
+      <c r="A11" s="15" t="s">
         <v>97</v>
       </c>
       <c r="B11" s="13" t="s">
@@ -1589,8 +1588,8 @@
       </c>
     </row>
     <row r="12" spans="1:10" ht="105" x14ac:dyDescent="0.25">
-      <c r="A12" s="17"/>
-      <c r="B12" s="14"/>
+      <c r="A12" s="16"/>
+      <c r="B12" s="18"/>
       <c r="C12" s="3" t="s">
         <v>50</v>
       </c>
@@ -1617,8 +1616,8 @@
       </c>
     </row>
     <row r="13" spans="1:10" ht="90" x14ac:dyDescent="0.25">
-      <c r="A13" s="17"/>
-      <c r="B13" s="14"/>
+      <c r="A13" s="16"/>
+      <c r="B13" s="18"/>
       <c r="C13" s="3" t="s">
         <v>55</v>
       </c>
@@ -1645,8 +1644,8 @@
       </c>
     </row>
     <row r="14" spans="1:10" ht="105" x14ac:dyDescent="0.25">
-      <c r="A14" s="18"/>
-      <c r="B14" s="15"/>
+      <c r="A14" s="19"/>
+      <c r="B14" s="14"/>
       <c r="C14" s="3" t="s">
         <v>56</v>
       </c>
@@ -1705,7 +1704,7 @@
       </c>
     </row>
     <row r="16" spans="1:10" ht="105" x14ac:dyDescent="0.25">
-      <c r="A16" s="16" t="s">
+      <c r="A16" s="15" t="s">
         <v>100</v>
       </c>
       <c r="B16" s="13" t="s">
@@ -1737,8 +1736,8 @@
       </c>
     </row>
     <row r="17" spans="1:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="A17" s="17"/>
-      <c r="B17" s="15"/>
+      <c r="A17" s="16"/>
+      <c r="B17" s="14"/>
       <c r="C17" s="3" t="s">
         <v>67</v>
       </c>
@@ -1763,7 +1762,7 @@
       </c>
     </row>
     <row r="18" spans="1:10" ht="90" x14ac:dyDescent="0.25">
-      <c r="A18" s="19" t="s">
+      <c r="A18" s="17" t="s">
         <v>102</v>
       </c>
       <c r="B18" s="13" t="s">
@@ -1795,8 +1794,8 @@
       </c>
     </row>
     <row r="19" spans="1:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="A19" s="19"/>
-      <c r="B19" s="14"/>
+      <c r="A19" s="17"/>
+      <c r="B19" s="18"/>
       <c r="C19" s="3" t="s">
         <v>75</v>
       </c>
@@ -1821,8 +1820,8 @@
       </c>
     </row>
     <row r="20" spans="1:10" ht="90" x14ac:dyDescent="0.25">
-      <c r="A20" s="19"/>
-      <c r="B20" s="15"/>
+      <c r="A20" s="17"/>
+      <c r="B20" s="14"/>
       <c r="C20" s="3" t="s">
         <v>80</v>
       </c>
@@ -1847,7 +1846,7 @@
       </c>
     </row>
     <row r="21" spans="1:10" ht="105" x14ac:dyDescent="0.25">
-      <c r="A21" s="19" t="s">
+      <c r="A21" s="17" t="s">
         <v>108</v>
       </c>
       <c r="B21" s="13" t="s">
@@ -1879,8 +1878,8 @@
       </c>
     </row>
     <row r="22" spans="1:10" ht="105" x14ac:dyDescent="0.25">
-      <c r="A22" s="19"/>
-      <c r="B22" s="14"/>
+      <c r="A22" s="17"/>
+      <c r="B22" s="18"/>
       <c r="C22" s="3" t="s">
         <v>105</v>
       </c>
@@ -1907,8 +1906,8 @@
       </c>
     </row>
     <row r="23" spans="1:10" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="19"/>
-      <c r="B23" s="15"/>
+      <c r="A23" s="17"/>
+      <c r="B23" s="14"/>
       <c r="C23" s="3" t="s">
         <v>89</v>
       </c>
@@ -1935,7 +1934,7 @@
       </c>
     </row>
     <row r="24" spans="1:10" ht="105" x14ac:dyDescent="0.25">
-      <c r="A24" s="19" t="s">
+      <c r="A24" s="17" t="s">
         <v>112</v>
       </c>
       <c r="B24" s="13" t="s">
@@ -1967,8 +1966,8 @@
       </c>
     </row>
     <row r="25" spans="1:10" ht="105" x14ac:dyDescent="0.25">
-      <c r="A25" s="19"/>
-      <c r="B25" s="14"/>
+      <c r="A25" s="17"/>
+      <c r="B25" s="18"/>
       <c r="C25" s="3" t="s">
         <v>113</v>
       </c>
@@ -1995,8 +1994,8 @@
       </c>
     </row>
     <row r="26" spans="1:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="A26" s="19"/>
-      <c r="B26" s="15"/>
+      <c r="A26" s="17"/>
+      <c r="B26" s="14"/>
       <c r="C26" s="3" t="s">
         <v>141</v>
       </c>
@@ -2024,6 +2023,12 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="B11:B14"/>
+    <mergeCell ref="A11:A14"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="A8:A10"/>
     <mergeCell ref="B16:B17"/>
     <mergeCell ref="A16:A17"/>
     <mergeCell ref="A24:A26"/>
@@ -2032,12 +2037,6 @@
     <mergeCell ref="A21:A23"/>
     <mergeCell ref="B18:B20"/>
     <mergeCell ref="A18:A20"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="B11:B14"/>
-    <mergeCell ref="A11:A14"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="A8:A10"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations count="1">

</xml_diff>